<commit_message>
integração com o pycharm
</commit_message>
<xml_diff>
--- a/Clientes.xlsx
+++ b/Clientes.xlsx
@@ -1,37 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -50,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -330,13 +385,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A2:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Diego Ferreira</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>123456</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Rua Candido das Laranjeiras</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nada consta!
+</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
mudança na pasta do excel
</commit_message>
<xml_diff>
--- a/Clientes.xlsx
+++ b/Clientes.xlsx
@@ -3,20 +3,20 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -24,16 +24,30 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -41,17 +55,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -134,44 +166,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -198,15 +230,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -233,7 +264,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -245,142 +275,166 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
@@ -390,14 +444,54 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="30.42578125" customWidth="1" min="1" max="1"/>
+    <col width="13.140625" customWidth="1" min="2" max="2"/>
+    <col width="6.85546875" customWidth="1" min="3" max="3"/>
+    <col width="10" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="26" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="41.85546875" customWidth="1" min="6" max="6"/>
+  </cols>
   <sheetData>
+    <row r="1" ht="19.5" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Nome completo</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Contato</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Idade</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Gênero</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Endereço</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Observações</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
@@ -406,7 +500,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>123456</t>
+          <t>12345</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -426,12 +520,46 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nada consta!
+          <t xml:space="preserve">Nada Consta!
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Alinny Raphaella</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>215456</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Rua José genuino</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Declarão de renda em análise!
 </t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>